<commit_message>
Delete Prediction, All In Karyawan
</commit_message>
<xml_diff>
--- a/public/template_karyawan.xlsx
+++ b/public/template_karyawan.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fadhilfn04/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fadhilfn04/Documents/Work/Projects/PUNDIRUPIAH/metronic_laravel_v8.2.6/prediksi-kinerja-karyawan/public/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{91168BCA-D2C1-674C-9628-C55547985C9B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AFC84096-FA6C-114C-93B9-27AECB5A7A37}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4180" yWindow="1500" windowWidth="28040" windowHeight="17440" xr2:uid="{9AC636AB-3F41-CD4D-B413-BB8CBF7D4A58}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>nik</t>
   </si>
@@ -72,6 +72,12 @@
   </si>
   <si>
     <t>Staff IT</t>
+  </si>
+  <si>
+    <t>umur</t>
+  </si>
+  <si>
+    <t>nilai_produktivitas</t>
   </si>
 </sst>
 </file>
@@ -443,15 +449,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0210CA1F-66A1-D94F-BC96-02ECA32ABD4B}">
-  <dimension ref="A1:H2"/>
+  <dimension ref="A1:J2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+      <selection activeCell="J10" sqref="J10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="10" max="10" width="30.6640625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -459,48 +468,60 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="H1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="I1" t="s">
+        <v>13</v>
+      </c>
+      <c r="J1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
-        <v>7</v>
-      </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1234567890</v>
       </c>
       <c r="B2" t="s">
         <v>8</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2">
+        <v>20</v>
+      </c>
+      <c r="D2" t="s">
         <v>9</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>10</v>
       </c>
-      <c r="E2">
+      <c r="F2" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2">
         <v>5</v>
       </c>
-      <c r="F2">
+      <c r="H2">
         <v>220</v>
       </c>
-      <c r="G2">
+      <c r="I2">
+        <v>70</v>
+      </c>
+      <c r="J2">
         <v>85</v>
-      </c>
-      <c r="H2" t="s">
-        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>